<commit_message>
Updated dependencies + consequences for scripts (e.g. array transposes), and added use of d18O_sw from Petryshyn paper for temperature calculation.
</commit_message>
<xml_diff>
--- a/Trudgill_et_al_202X/Data/TJ_d18O_d13C.xlsx
+++ b/Trudgill_et_al_202X/Data/TJ_d18O_d13C.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="340">
   <si>
     <t>Height</t>
   </si>
@@ -795,6 +795,132 @@
   </si>
   <si>
     <t>anderson_arthur_temperature</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>‰</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>oneil_temperature</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature</t>
+  </si>
+  <si>
+    <t>hansen_temperature</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>‰</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>d13C_uncertainty</t>
+  </si>
+  <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>d18O_uncertainty</t>
+  </si>
+  <si>
+    <t>oneil_temperature</t>
+  </si>
+  <si>
+    <t>oneil_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>hansen_temperature</t>
+  </si>
+  <si>
+    <t>hansen_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>‰</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>d13C_uncertainty</t>
+  </si>
+  <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>d18O_uncertainty</t>
+  </si>
+  <si>
+    <t>delta_temperature</t>
+  </si>
+  <si>
+    <t>delta_temperature_uncertainty</t>
   </si>
   <si>
     <t>m</t>
@@ -956,7 +1082,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="55">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -1018,11 +1144,20 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -1080,6 +1215,15 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5850,7 +5994,7 @@
     <col min="3" max="3" width="4.7109375" customWidth="true"/>
     <col min="4" max="4" width="5.37890625" customWidth="true"/>
     <col min="5" max="5" width="11.7109375" customWidth="true"/>
-    <col min="7" max="7" width="5.7109375" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
     <col min="8" max="8" width="9.7109375" customWidth="true"/>
     <col min="2" max="2" width="11.7109375" customWidth="true"/>
     <col min="6" max="6" width="11.7109375" customWidth="true"/>
@@ -5858,54 +6002,54 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.3">
       <c r="A1" s="0" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>257</v>
+        <v>299</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>258</v>
+        <v>300</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>259</v>
+        <v>301</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>260</v>
+        <v>302</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>261</v>
+        <v>303</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>262</v>
+        <v>304</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>263</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.3">
       <c r="A2" s="0" t="s">
-        <v>264</v>
+        <v>306</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>265</v>
+        <v>307</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>266</v>
+        <v>308</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>266</v>
+        <v>308</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.3">
@@ -5928,7 +6072,7 @@
         <v>10.121146595580001</v>
       </c>
       <c r="G3" s="0">
-        <v>13.68</v>
+        <v>22.693090909090909</v>
       </c>
       <c r="H3" s="0">
         <v>12.849891999999999</v>
@@ -5954,7 +6098,7 @@
         <v>6.2581917692353386</v>
       </c>
       <c r="G4" s="0">
-        <v>10.16</v>
+        <v>19.173090909090909</v>
       </c>
       <c r="H4" s="0">
         <v>9.4858280000000015</v>
@@ -5980,7 +6124,7 @@
         <v>9.9876404466590998</v>
       </c>
       <c r="G5" s="0">
-        <v>13.56</v>
+        <v>22.573090909090908</v>
       </c>
       <c r="H5" s="0">
         <v>12.731892999999999</v>
@@ -6006,7 +6150,7 @@
         <v>9.0567208156062975</v>
       </c>
       <c r="G6" s="0">
-        <v>12.720000000000001</v>
+        <v>21.733090909090908</v>
       </c>
       <c r="H6" s="0">
         <v>11.912452</v>
@@ -6032,7 +6176,7 @@
         <v>8.6596860360670576</v>
       </c>
       <c r="G7" s="0">
-        <v>12.359999999999999</v>
+        <v>21.373090909090909</v>
       </c>
       <c r="H7" s="0">
         <v>11.564773000000002</v>
@@ -6058,7 +6202,7 @@
         <v>8.7919028052227759</v>
       </c>
       <c r="G8" s="0">
-        <v>12.48</v>
+        <v>21.49309090909091</v>
       </c>
       <c r="H8" s="0">
         <v>11.680432</v>
@@ -6084,7 +6228,7 @@
         <v>4.4525766425982169</v>
       </c>
       <c r="G9" s="0">
-        <v>8.4800000000000004</v>
+        <v>17.49309090909091</v>
       </c>
       <c r="H9" s="0">
         <v>7.9512320000000001</v>
@@ -6110,7 +6254,7 @@
         <v>8.7037440711314389</v>
       </c>
       <c r="G10" s="0">
-        <v>12.4</v>
+        <v>21.413090909090911</v>
       </c>
       <c r="H10" s="0">
         <v>11.603300000000001</v>
@@ -6136,7 +6280,7 @@
         <v>9.7654185162721774</v>
       </c>
       <c r="G11" s="0">
-        <v>13.359999999999999</v>
+        <v>22.373090909090909</v>
       </c>
       <c r="H11" s="0">
         <v>12.535748</v>
@@ -6162,7 +6306,7 @@
         <v>4.1113777368287856</v>
       </c>
       <c r="G12" s="0">
-        <v>8.1600000000000001</v>
+        <v>17.173090909090909</v>
       </c>
       <c r="H12" s="0">
         <v>7.6641280000000007</v>
@@ -6188,7 +6332,7 @@
         <v>5.869235598726732</v>
       </c>
       <c r="G13" s="0">
-        <v>9.8000000000000007</v>
+        <v>18.81309090909091</v>
       </c>
       <c r="H13" s="0">
         <v>9.1531250000000011</v>
@@ -6214,7 +6358,7 @@
         <v>7.4318061575210663</v>
       </c>
       <c r="G14" s="0">
-        <v>11.24</v>
+        <v>20.253090909090908</v>
       </c>
       <c r="H14" s="0">
         <v>10.496573</v>
@@ -6240,7 +6384,7 @@
         <v>8.7919028052227759</v>
       </c>
       <c r="G15" s="0">
-        <v>12.48</v>
+        <v>21.49309090909091</v>
       </c>
       <c r="H15" s="0">
         <v>11.680432</v>
@@ -6266,7 +6410,7 @@
         <v>1.3291863169953899</v>
       </c>
       <c r="G16" s="0">
-        <v>5.5199999999999996</v>
+        <v>14.533090909090909</v>
       </c>
       <c r="H16" s="0">
         <v>5.3590120000000008</v>
@@ -6292,7 +6436,7 @@
         <v>8.0882223861275406</v>
       </c>
       <c r="G17" s="0">
-        <v>11.84</v>
+        <v>20.853090909090909</v>
       </c>
       <c r="H17" s="0">
         <v>11.066288</v>
@@ -6318,7 +6462,7 @@
         <v>10.433166728444291</v>
       </c>
       <c r="G18" s="0">
-        <v>13.960000000000001</v>
+        <v>22.97309090909091</v>
       </c>
       <c r="H18" s="0">
         <v>13.126133000000001</v>
@@ -6344,7 +6488,7 @@
         <v>6.7351055745222652</v>
       </c>
       <c r="G19" s="0">
-        <v>10.6</v>
+        <v>19.613090909090911</v>
       </c>
       <c r="H19" s="0">
         <v>9.8953250000000015</v>
@@ -6370,7 +6514,7 @@
         <v>7.9128682990457833</v>
       </c>
       <c r="G20" s="0">
-        <v>11.68</v>
+        <v>20.693090909090909</v>
       </c>
       <c r="H20" s="0">
         <v>10.913792000000001</v>
@@ -6396,7 +6540,7 @@
         <v>8.4835959484826731</v>
       </c>
       <c r="G21" s="0">
-        <v>12.199999999999999</v>
+        <v>21.213090909090909</v>
       </c>
       <c r="H21" s="0">
         <v>11.410925000000001</v>
@@ -6422,7 +6566,7 @@
         <v>8.4835959484826731</v>
       </c>
       <c r="G22" s="0">
-        <v>12.199999999999999</v>
+        <v>21.213090909090909</v>
       </c>
       <c r="H22" s="0">
         <v>11.410925000000001</v>
@@ -6448,7 +6592,7 @@
         <v>8.4835959484826731</v>
       </c>
       <c r="G23" s="0">
-        <v>12.199999999999999</v>
+        <v>21.213090909090909</v>
       </c>
       <c r="H23" s="0">
         <v>11.410925000000001</v>
@@ -6474,7 +6618,7 @@
         <v>8.4835959484826731</v>
       </c>
       <c r="G24" s="0">
-        <v>12.199999999999999</v>
+        <v>21.213090909090909</v>
       </c>
       <c r="H24" s="0">
         <v>11.410925000000001</v>
@@ -6500,7 +6644,7 @@
         <v>7.5191455463768762</v>
       </c>
       <c r="G25" s="0">
-        <v>11.32</v>
+        <v>20.33309090909091</v>
       </c>
       <c r="H25" s="0">
         <v>10.572197000000001</v>
@@ -6526,7 +6670,7 @@
         <v>8.1759841408550642</v>
       </c>
       <c r="G26" s="0">
-        <v>11.92</v>
+        <v>20.933090909090907</v>
       </c>
       <c r="H26" s="0">
         <v>11.142692</v>
@@ -6552,7 +6696,7 @@
         <v>11.868623742659679</v>
       </c>
       <c r="G27" s="0">
-        <v>15.24</v>
+        <v>24.253090909090908</v>
       </c>
       <c r="H27" s="0">
         <v>14.405173000000001</v>
@@ -6578,7 +6722,7 @@
         <v>11.149025847176517</v>
       </c>
       <c r="G28" s="0">
-        <v>14.6</v>
+        <v>23.613090909090907</v>
       </c>
       <c r="H28" s="0">
         <v>13.762325000000001</v>
@@ -6604,7 +6748,7 @@
         <v>12.81881913113574</v>
       </c>
       <c r="G29" s="0">
-        <v>16.079999999999998</v>
+        <v>25.093090909090911</v>
       </c>
       <c r="H29" s="0">
         <v>15.259012</v>
@@ -6630,7 +6774,7 @@
         <v>9.8542640828106869</v>
       </c>
       <c r="G30" s="0">
-        <v>13.44</v>
+        <v>22.453090909090911</v>
       </c>
       <c r="H30" s="0">
         <v>12.614128000000001</v>
@@ -6656,7 +6800,7 @@
         <v>12.139442842778919</v>
       </c>
       <c r="G31" s="0">
-        <v>15.48</v>
+        <v>24.49309090909091</v>
       </c>
       <c r="H31" s="0">
         <v>14.647957000000002</v>
@@ -6682,7 +6826,7 @@
         <v>11.823538785435005</v>
       </c>
       <c r="G32" s="0">
-        <v>15.199999999999999</v>
+        <v>24.213090909090909</v>
       </c>
       <c r="H32" s="0">
         <v>14.364800000000001</v>
@@ -6708,7 +6852,7 @@
         <v>11.823538785435005</v>
       </c>
       <c r="G33" s="0">
-        <v>15.199999999999999</v>
+        <v>24.213090909090909</v>
       </c>
       <c r="H33" s="0">
         <v>14.364800000000001</v>
@@ -6734,7 +6878,7 @@
         <v>11.193890877900003</v>
       </c>
       <c r="G34" s="0">
-        <v>14.640000000000001</v>
+        <v>23.65309090909091</v>
       </c>
       <c r="H34" s="0">
         <v>13.802308</v>
@@ -6760,7 +6904,7 @@
         <v>9.7654185162721774</v>
       </c>
       <c r="G35" s="0">
-        <v>13.359999999999999</v>
+        <v>22.373090909090909</v>
       </c>
       <c r="H35" s="0">
         <v>12.535748</v>
@@ -6786,7 +6930,7 @@
         <v>10.388549007356119</v>
       </c>
       <c r="G36" s="0">
-        <v>13.92</v>
+        <v>22.933090909090907</v>
       </c>
       <c r="H36" s="0">
         <v>13.086592000000001</v>
@@ -6812,7 +6956,7 @@
         <v>13.000550249830894</v>
       </c>
       <c r="G37" s="0">
-        <v>16.240000000000002</v>
+        <v>25.253090909090908</v>
       </c>
       <c r="H37" s="0">
         <v>15.422948000000002</v>
@@ -6838,7 +6982,7 @@
         <v>7.300902216570023</v>
       </c>
       <c r="G38" s="0">
-        <v>11.119999999999999</v>
+        <v>20.13309090909091</v>
       </c>
       <c r="H38" s="0">
         <v>10.383332000000001</v>
@@ -6864,7 +7008,7 @@
         <v>12.410793396579948</v>
       </c>
       <c r="G39" s="0">
-        <v>15.720000000000001</v>
+        <v>24.733090909090912</v>
       </c>
       <c r="H39" s="0">
         <v>14.891677000000001</v>
@@ -6890,7 +7034,7 @@
         <v>13.501541569385154</v>
       </c>
       <c r="G40" s="0">
-        <v>16.68</v>
+        <v>25.693090909090909</v>
       </c>
       <c r="H40" s="0">
         <v>15.875916999999999</v>
@@ -6916,7 +7060,7 @@
         <v>13.501541569385154</v>
       </c>
       <c r="G41" s="0">
-        <v>16.68</v>
+        <v>25.693090909090909</v>
       </c>
       <c r="H41" s="0">
         <v>15.875916999999999</v>
@@ -6942,7 +7086,7 @@
         <v>13.137005023359677</v>
       </c>
       <c r="G42" s="0">
-        <v>16.359999999999999</v>
+        <v>25.373090909090909</v>
       </c>
       <c r="H42" s="0">
         <v>15.546173000000001</v>
@@ -6968,7 +7112,7 @@
         <v>13.547175978628218</v>
       </c>
       <c r="G43" s="0">
-        <v>16.719999999999999</v>
+        <v>25.733090909090908</v>
       </c>
       <c r="H43" s="0">
         <v>15.917252</v>
@@ -6994,7 +7138,7 @@
         <v>13.867036956401535</v>
       </c>
       <c r="G44" s="0">
-        <v>17</v>
+        <v>26.013090909090909</v>
       </c>
       <c r="H44" s="0">
         <v>16.207325000000001</v>
@@ -7020,7 +7164,7 @@
         <v>13.547175978628218</v>
       </c>
       <c r="G45" s="0">
-        <v>16.719999999999999</v>
+        <v>25.733090909090908</v>
       </c>
       <c r="H45" s="0">
         <v>15.917252</v>
@@ -7046,7 +7190,7 @@
         <v>9.9431672474979109</v>
       </c>
       <c r="G46" s="0">
-        <v>13.52</v>
+        <v>22.533090909090909</v>
       </c>
       <c r="H46" s="0">
         <v>12.692612</v>
@@ -7072,7 +7216,7 @@
         <v>9.9431672474979109</v>
       </c>
       <c r="G47" s="0">
-        <v>13.52</v>
+        <v>22.533090909090909</v>
       </c>
       <c r="H47" s="0">
         <v>12.692612</v>
@@ -7098,7 +7242,7 @@
         <v>11.91372341913177</v>
       </c>
       <c r="G48" s="0">
-        <v>15.279999999999999</v>
+        <v>24.293090909090907</v>
       </c>
       <c r="H48" s="0">
         <v>14.445572</v>
@@ -7124,7 +7268,7 @@
         <v>10.165677519104634</v>
       </c>
       <c r="G49" s="0">
-        <v>13.720000000000001</v>
+        <v>22.733090909090908</v>
       </c>
       <c r="H49" s="0">
         <v>12.889277</v>
@@ -7150,7 +7294,7 @@
         <v>9.3220526992475925</v>
       </c>
       <c r="G50" s="0">
-        <v>12.960000000000001</v>
+        <v>21.97309090909091</v>
       </c>
       <c r="H50" s="0">
         <v>12.145408000000002</v>
@@ -7176,7 +7320,7 @@
         <v>9.4549118113342843</v>
       </c>
       <c r="G51" s="0">
-        <v>13.08</v>
+        <v>22.093090909090911</v>
       </c>
       <c r="H51" s="0">
         <v>12.262237000000001</v>
@@ -7202,7 +7346,7 @@
         <v>7.5628362895495798</v>
       </c>
       <c r="G52" s="0">
-        <v>11.359999999999999</v>
+        <v>20.373090909090909</v>
       </c>
       <c r="H52" s="0">
         <v>10.610048000000003</v>
@@ -7228,7 +7372,7 @@
         <v>10.299357009765174</v>
       </c>
       <c r="G53" s="0">
-        <v>13.84</v>
+        <v>22.853090909090909</v>
       </c>
       <c r="H53" s="0">
         <v>13.007588</v>
@@ -7254,7 +7398,7 @@
         <v>10.656472839284788</v>
       </c>
       <c r="G54" s="0">
-        <v>14.16</v>
+        <v>23.173090909090909</v>
       </c>
       <c r="H54" s="0">
         <v>13.324228000000002</v>
@@ -7280,7 +7424,7 @@
         <v>10.656472839284788</v>
       </c>
       <c r="G55" s="0">
-        <v>14.16</v>
+        <v>23.173090909090909</v>
       </c>
       <c r="H55" s="0">
         <v>13.324228000000002</v>
@@ -7306,7 +7450,7 @@
         <v>13.59282537712113</v>
       </c>
       <c r="G56" s="0">
-        <v>16.759999999999998</v>
+        <v>25.773090909090911</v>
       </c>
       <c r="H56" s="0">
         <v>15.958613</v>
@@ -7332,7 +7476,7 @@
         <v>12.955095137022226</v>
       </c>
       <c r="G57" s="0">
-        <v>16.199999999999999</v>
+        <v>25.213090909090909</v>
       </c>
       <c r="H57" s="0">
         <v>15.381925000000001</v>
@@ -7358,7 +7502,7 @@
         <v>16.359501785799466</v>
       </c>
       <c r="G58" s="0">
-        <v>19.16</v>
+        <v>28.173090909090909</v>
       </c>
       <c r="H58" s="0">
         <v>18.487852999999998</v>
@@ -7384,7 +7528,7 @@
         <v>13.867036956401535</v>
       </c>
       <c r="G59" s="0">
-        <v>17</v>
+        <v>26.013090909090909</v>
       </c>
       <c r="H59" s="0">
         <v>16.207325000000001</v>
@@ -7410,7 +7554,7 @@
         <v>11.328573668453544</v>
       </c>
       <c r="G60" s="0">
-        <v>14.76</v>
+        <v>23.773090909090911</v>
       </c>
       <c r="H60" s="0">
         <v>13.922413000000001</v>
@@ -7436,7 +7580,7 @@
         <v>13.137005023359677</v>
       </c>
       <c r="G61" s="0">
-        <v>16.359999999999999</v>
+        <v>25.373090909090909</v>
       </c>
       <c r="H61" s="0">
         <v>15.546173000000001</v>
@@ -7462,7 +7606,7 @@
         <v>13.000550249830894</v>
       </c>
       <c r="G62" s="0">
-        <v>16.240000000000002</v>
+        <v>25.253090909090908</v>
       </c>
       <c r="H62" s="0">
         <v>15.422948000000002</v>
@@ -7488,7 +7632,7 @@
         <v>16.312939334260875</v>
       </c>
       <c r="G63" s="0">
-        <v>19.120000000000001</v>
+        <v>28.13309090909091</v>
       </c>
       <c r="H63" s="0">
         <v>18.444931999999998</v>
@@ -7514,7 +7658,7 @@
         <v>16.126843864334433</v>
       </c>
       <c r="G64" s="0">
-        <v>18.960000000000001</v>
+        <v>27.97309090909091</v>
       </c>
       <c r="H64" s="0">
         <v>18.273508</v>
@@ -7540,7 +7684,7 @@
         <v>12.591989791107039</v>
       </c>
       <c r="G65" s="0">
-        <v>15.879999999999999</v>
+        <v>24.893090909090908</v>
       </c>
       <c r="H65" s="0">
         <v>15.054677</v>
@@ -7566,7 +7710,7 @@
         <v>8.5275971762246741</v>
       </c>
       <c r="G66" s="0">
-        <v>12.24</v>
+        <v>21.253090909090908</v>
       </c>
       <c r="H66" s="0">
         <v>11.449348000000001</v>
@@ -7592,7 +7736,7 @@
         <v>12.682676970470027</v>
       </c>
       <c r="G67" s="0">
-        <v>15.960000000000001</v>
+        <v>24.97309090909091</v>
       </c>
       <c r="H67" s="0">
         <v>15.136332999999999</v>
@@ -7618,7 +7762,7 @@
         <v>14.831052186376382</v>
       </c>
       <c r="G68" s="0">
-        <v>17.84</v>
+        <v>26.853090909090909</v>
       </c>
       <c r="H68" s="0">
         <v>17.085187999999999</v>
@@ -7644,7 +7788,7 @@
         <v>13.273594103638004</v>
       </c>
       <c r="G69" s="0">
-        <v>16.48</v>
+        <v>25.49309090909091</v>
       </c>
       <c r="H69" s="0">
         <v>15.669632000000002</v>
@@ -7670,7 +7814,7 @@
         <v>12.229833899742857</v>
       </c>
       <c r="G70" s="0">
-        <v>15.56</v>
+        <v>24.573090909090908</v>
       </c>
       <c r="H70" s="0">
         <v>14.729092999999999</v>
@@ -7696,7 +7840,7 @@
         <v>15.107713110195107</v>
       </c>
       <c r="G71" s="0">
-        <v>18.079999999999998</v>
+        <v>27.093090909090911</v>
       </c>
       <c r="H71" s="0">
         <v>17.338111999999999</v>
@@ -7722,7 +7866,7 @@
         <v>14.600919430280271</v>
       </c>
       <c r="G72" s="0">
-        <v>17.640000000000001</v>
+        <v>26.65309090909091</v>
       </c>
       <c r="H72" s="0">
         <v>16.875132999999998</v>
@@ -7748,7 +7892,7 @@
         <v>17.575570711350906</v>
       </c>
       <c r="G73" s="0">
-        <v>20.199999999999999</v>
+        <v>29.213090909090909</v>
       </c>
       <c r="H73" s="0">
         <v>19.612924999999997</v>
@@ -7774,7 +7918,7 @@
         <v>17.481653076924601</v>
       </c>
       <c r="G74" s="0">
-        <v>20.119999999999997</v>
+        <v>29.13309090909091</v>
       </c>
       <c r="H74" s="0">
         <v>19.525756999999999</v>
@@ -7800,7 +7944,7 @@
         <v>13.82129746708523</v>
       </c>
       <c r="G75" s="0">
-        <v>16.960000000000001</v>
+        <v>25.97309090909091</v>
       </c>
       <c r="H75" s="0">
         <v>16.165808000000002</v>
@@ -7826,7 +7970,7 @@
         <v>16.359501785799466</v>
       </c>
       <c r="G76" s="0">
-        <v>19.16</v>
+        <v>28.173090909090909</v>
       </c>
       <c r="H76" s="0">
         <v>18.487852999999998</v>
@@ -7852,7 +7996,7 @@
         <v>16.779259978342679</v>
       </c>
       <c r="G77" s="0">
-        <v>19.52</v>
+        <v>28.533090909090909</v>
       </c>
       <c r="H77" s="0">
         <v>18.875312000000001</v>
@@ -7878,7 +8022,7 @@
         <v>14.508972503349014</v>
       </c>
       <c r="G78" s="0">
-        <v>17.559999999999999</v>
+        <v>26.573090909090908</v>
       </c>
       <c r="H78" s="0">
         <v>16.791293</v>
@@ -7904,7 +8048,7 @@
         <v>14.508972503349014</v>
       </c>
       <c r="G79" s="0">
-        <v>17.559999999999999</v>
+        <v>26.573090909090908</v>
       </c>
       <c r="H79" s="0">
         <v>16.791293</v>
@@ -7930,7 +8074,7 @@
         <v>14.508972503349014</v>
       </c>
       <c r="G80" s="0">
-        <v>17.559999999999999</v>
+        <v>26.573090909090908</v>
       </c>
       <c r="H80" s="0">
         <v>16.791293</v>
@@ -7956,7 +8100,7 @@
         <v>14.508972503349014</v>
       </c>
       <c r="G81" s="0">
-        <v>17.559999999999999</v>
+        <v>26.573090909090908</v>
       </c>
       <c r="H81" s="0">
         <v>16.791293</v>
@@ -7995,90 +8139,90 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.3">
       <c r="A1" s="0" t="s">
-        <v>268</v>
+        <v>310</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>269</v>
+        <v>311</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>270</v>
+        <v>312</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>271</v>
+        <v>313</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>272</v>
+        <v>314</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>273</v>
+        <v>315</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>274</v>
+        <v>316</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>276</v>
+        <v>318</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>278</v>
+        <v>320</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>279</v>
+        <v>321</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>280</v>
+        <v>322</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>281</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.3">
       <c r="A2" s="0" t="s">
-        <v>282</v>
+        <v>324</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>283</v>
+        <v>325</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>284</v>
+        <v>326</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>284</v>
+        <v>326</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>284</v>
+        <v>326</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>284</v>
+        <v>326</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>285</v>
+        <v>327</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>285</v>
+        <v>327</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>285</v>
+        <v>327</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>285</v>
+        <v>327</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>285</v>
+        <v>327</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>285</v>
+        <v>327</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>285</v>
+        <v>327</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>285</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.3">
@@ -8113,10 +8257,10 @@
         <v>1.7953739105371873</v>
       </c>
       <c r="K3" s="0">
-        <v>12.529999999999999</v>
+        <v>21.543090909090907</v>
       </c>
       <c r="L3" s="0">
-        <v>1.6367040050051813</v>
+        <v>1.6367040050051809</v>
       </c>
       <c r="M3" s="0">
         <v>11.745016250000001</v>
@@ -8157,7 +8301,7 @@
         <v>2.3225707626472936</v>
       </c>
       <c r="K4" s="0">
-        <v>11.005714285714285</v>
+        <v>20.018805194805193</v>
       </c>
       <c r="L4" s="0">
         <v>2.1379652097485677</v>
@@ -8201,7 +8345,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K5" s="0">
-        <v>10.27</v>
+        <v>19.283090909090909</v>
       </c>
       <c r="L5" s="0">
         <v>3.2068884192209333</v>
@@ -8245,10 +8389,10 @@
         <v>2.6149241191808139</v>
       </c>
       <c r="K6" s="0">
-        <v>12.280000000000001</v>
+        <v>21.29309090909091</v>
       </c>
       <c r="L6" s="0">
-        <v>2.3758787847868006</v>
+        <v>2.3758787847867993</v>
       </c>
       <c r="M6" s="0">
         <v>11.510729000000001</v>
@@ -8289,7 +8433,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K7" s="0">
-        <v>11.68</v>
+        <v>20.693090909090909</v>
       </c>
       <c r="L7" s="0">
         <v>3.2068884192209333</v>
@@ -8333,7 +8477,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K8" s="0">
-        <v>12.199999999999999</v>
+        <v>21.213090909090909</v>
       </c>
       <c r="L8" s="0">
         <v>3.2068884192209333</v>
@@ -8377,10 +8521,10 @@
         <v>0.46445502430056751</v>
       </c>
       <c r="K9" s="0">
-        <v>11.620000000000001</v>
+        <v>20.63309090909091</v>
       </c>
       <c r="L9" s="0">
-        <v>0.42426406871192823</v>
+        <v>0.42426406871192701</v>
       </c>
       <c r="M9" s="0">
         <v>10.8574445</v>
@@ -8421,10 +8565,10 @@
         <v>1.2493845657916447</v>
       </c>
       <c r="K10" s="0">
-        <v>14.84</v>
+        <v>23.853090909090909</v>
       </c>
       <c r="L10" s="0">
-        <v>1.112834219459484</v>
+        <v>1.1128342194594845</v>
       </c>
       <c r="M10" s="0">
         <v>14.0101595</v>
@@ -8465,7 +8609,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K11" s="0">
-        <v>15.48</v>
+        <v>24.49309090909091</v>
       </c>
       <c r="L11" s="0">
         <v>3.2068884192209333</v>
@@ -8509,10 +8653,10 @@
         <v>1.151575452677519</v>
       </c>
       <c r="K12" s="0">
-        <v>14.76</v>
+        <v>23.773090909090907</v>
       </c>
       <c r="L12" s="0">
-        <v>1.0254364924265185</v>
+        <v>1.0254364924265176</v>
       </c>
       <c r="M12" s="0">
         <v>13.929532666666667</v>
@@ -8553,7 +8697,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K13" s="0">
-        <v>11.119999999999999</v>
+        <v>20.13309090909091</v>
       </c>
       <c r="L13" s="0">
         <v>3.2068884192209333</v>
@@ -8597,7 +8741,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K14" s="0">
-        <v>15.720000000000001</v>
+        <v>24.733090909090912</v>
       </c>
       <c r="L14" s="0">
         <v>3.2068884192209333</v>
@@ -8641,7 +8785,7 @@
         <v>0.19108876600858454</v>
       </c>
       <c r="K15" s="0">
-        <v>16.609999999999999</v>
+        <v>25.623090909090909</v>
       </c>
       <c r="L15" s="0">
         <v>0.1677299416721216</v>
@@ -8685,7 +8829,7 @@
         <v>0.22617586642047185</v>
       </c>
       <c r="K16" s="0">
-        <v>16.859999999999999</v>
+        <v>25.873090909090909</v>
       </c>
       <c r="L16" s="0">
         <v>0.1979898987322341</v>
@@ -8729,7 +8873,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K17" s="0">
-        <v>13.52</v>
+        <v>22.533090909090909</v>
       </c>
       <c r="L17" s="0">
         <v>3.2068884192209333</v>
@@ -8773,7 +8917,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K18" s="0">
-        <v>15.279999999999999</v>
+        <v>24.293090909090907</v>
       </c>
       <c r="L18" s="0">
         <v>3.2068884192209333</v>
@@ -8817,10 +8961,10 @@
         <v>0.59653283089819331</v>
       </c>
       <c r="K19" s="0">
-        <v>13.34</v>
+        <v>22.353090909090909</v>
       </c>
       <c r="L19" s="0">
-        <v>0.53740115370177599</v>
+        <v>0.53740115370177477</v>
       </c>
       <c r="M19" s="0">
         <v>12.517342500000002</v>
@@ -8861,10 +9005,10 @@
         <v>1.3378994319710398</v>
       </c>
       <c r="K20" s="0">
-        <v>12.219999999999999</v>
+        <v>21.233090909090912</v>
       </c>
       <c r="L20" s="0">
-        <v>1.2162236636408621</v>
+        <v>1.2162236636408634</v>
       </c>
       <c r="M20" s="0">
         <v>11.436142500000003</v>
@@ -8905,7 +9049,7 @@
         <v>0.20618092030502574</v>
       </c>
       <c r="K21" s="0">
-        <v>14.053333333333333</v>
+        <v>23.066424242424244</v>
       </c>
       <c r="L21" s="0">
         <v>0.18475208614068039</v>
@@ -8949,10 +9093,10 @@
         <v>0.45094337734165996</v>
       </c>
       <c r="K22" s="0">
-        <v>16.479999999999997</v>
+        <v>25.49309090909091</v>
       </c>
       <c r="L22" s="0">
-        <v>0.39597979746446571</v>
+        <v>0.39597979746446821</v>
       </c>
       <c r="M22" s="0">
         <v>15.670269000000001</v>
@@ -8993,7 +9137,7 @@
         <v>1.7624387827362489</v>
       </c>
       <c r="K23" s="0">
-        <v>18.079999999999998</v>
+        <v>27.093090909090911</v>
       </c>
       <c r="L23" s="0">
         <v>1.5273506473629428</v>
@@ -9037,7 +9181,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K24" s="0">
-        <v>14.76</v>
+        <v>23.773090909090911</v>
       </c>
       <c r="L24" s="0">
         <v>3.2068884192209333</v>
@@ -9081,10 +9225,10 @@
         <v>0.096488095687476974</v>
       </c>
       <c r="K25" s="0">
-        <v>16.300000000000001</v>
+        <v>25.31309090909091</v>
       </c>
       <c r="L25" s="0">
-        <v>0.08485281374238389</v>
+        <v>0.084852813742386402</v>
       </c>
       <c r="M25" s="0">
         <v>15.484560500000001</v>
@@ -9125,7 +9269,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K26" s="0">
-        <v>19.120000000000001</v>
+        <v>28.13309090909091</v>
       </c>
       <c r="L26" s="0">
         <v>3.2068884192209333</v>
@@ -9169,7 +9313,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K27" s="0">
-        <v>18.960000000000001</v>
+        <v>27.97309090909091</v>
       </c>
       <c r="L27" s="0">
         <v>3.2068884192209333</v>
@@ -9213,10 +9357,10 @@
         <v>2.8739595793878441</v>
       </c>
       <c r="K28" s="0">
-        <v>14.059999999999999</v>
+        <v>23.073090909090908</v>
       </c>
       <c r="L28" s="0">
-        <v>2.5738686835190321</v>
+        <v>2.5738686835190334</v>
       </c>
       <c r="M28" s="0">
         <v>13.252012499999999</v>
@@ -9257,7 +9401,7 @@
         <v>1.1098329308263208</v>
       </c>
       <c r="K29" s="0">
-        <v>16.760000000000002</v>
+        <v>25.773090909090911</v>
       </c>
       <c r="L29" s="0">
         <v>0.9707728879609272</v>
@@ -9301,7 +9445,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K30" s="0">
-        <v>15.56</v>
+        <v>24.573090909090908</v>
       </c>
       <c r="L30" s="0">
         <v>3.2068884192209333</v>
@@ -9345,7 +9489,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K31" s="0">
-        <v>18.079999999999998</v>
+        <v>27.093090909090911</v>
       </c>
       <c r="L31" s="0">
         <v>3.2068884192209333</v>
@@ -9389,7 +9533,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K32" s="0">
-        <v>17.640000000000001</v>
+        <v>26.65309090909091</v>
       </c>
       <c r="L32" s="0">
         <v>3.2068884192209333</v>
@@ -9433,7 +9577,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K33" s="0">
-        <v>20.199999999999999</v>
+        <v>29.213090909090909</v>
       </c>
       <c r="L33" s="0">
         <v>3.2068884192209333</v>
@@ -9477,10 +9621,10 @@
         <v>2.5882622732716398</v>
       </c>
       <c r="K34" s="0">
-        <v>18.539999999999999</v>
+        <v>27.553090909090912</v>
       </c>
       <c r="L34" s="0">
-        <v>2.2344574285494878</v>
+        <v>2.2344574285494905</v>
       </c>
       <c r="M34" s="0">
         <v>17.845782499999999</v>
@@ -9521,7 +9665,7 @@
         <v>3.4326203083304709</v>
       </c>
       <c r="K35" s="0">
-        <v>19.16</v>
+        <v>28.173090909090909</v>
       </c>
       <c r="L35" s="0">
         <v>3.2068884192209333</v>
@@ -9565,7 +9709,7 @@
         <v>1.015303424510438</v>
       </c>
       <c r="K36" s="0">
-        <v>17.952000000000002</v>
+        <v>26.965090909090907</v>
       </c>
       <c r="L36" s="0">
         <v>0.87653864717991792</v>
@@ -9599,54 +9743,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>286</v>
+        <v>328</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>287</v>
+        <v>329</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>288</v>
+        <v>330</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>289</v>
+        <v>331</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>290</v>
+        <v>332</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>291</v>
+        <v>333</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>292</v>
+        <v>334</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>293</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>294</v>
+        <v>336</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>295</v>
+        <v>337</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>296</v>
+        <v>338</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>296</v>
+        <v>338</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>296</v>
+        <v>338</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>296</v>
+        <v>338</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3">
@@ -9672,7 +9816,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="0">
-        <v>1.6367040050051813</v>
+        <v>1.6367040050051809</v>
       </c>
     </row>
     <row r="4">
@@ -9721,7 +9865,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G5" s="0">
-        <v>-2.2599999999999998</v>
+        <v>-2.259999999999998</v>
       </c>
       <c r="H5" s="0">
         <v>3.2068884192209333</v>
@@ -9747,10 +9891,10 @@
         <v>0.59396969619669993</v>
       </c>
       <c r="G6" s="0">
-        <v>-0.24999999999999822</v>
+        <v>-0.24999999999999645</v>
       </c>
       <c r="H6" s="0">
-        <v>2.3758787847868006</v>
+        <v>2.3758787847867993</v>
       </c>
     </row>
     <row r="7">
@@ -9773,7 +9917,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G7" s="0">
-        <v>-0.84999999999999964</v>
+        <v>-0.84999999999999787</v>
       </c>
       <c r="H7" s="0">
         <v>3.2068884192209333</v>
@@ -9799,7 +9943,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G8" s="0">
-        <v>-0.33000000000000007</v>
+        <v>-0.32999999999999829</v>
       </c>
       <c r="H8" s="0">
         <v>3.2068884192209333</v>
@@ -9825,10 +9969,10 @@
         <v>0.10606601717798214</v>
       </c>
       <c r="G9" s="0">
-        <v>-0.90999999999999837</v>
+        <v>-0.90999999999999659</v>
       </c>
       <c r="H9" s="0">
-        <v>0.42426406871192823</v>
+        <v>0.42426406871192701</v>
       </c>
     </row>
     <row r="10">
@@ -9851,10 +9995,10 @@
         <v>0.27820855486487112</v>
       </c>
       <c r="G10" s="0">
-        <v>2.3100000000000005</v>
+        <v>2.3100000000000023</v>
       </c>
       <c r="H10" s="0">
-        <v>1.112834219459484</v>
+        <v>1.1128342194594845</v>
       </c>
     </row>
     <row r="11">
@@ -9877,7 +10021,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G11" s="0">
-        <v>2.9500000000000011</v>
+        <v>2.9500000000000028</v>
       </c>
       <c r="H11" s="0">
         <v>3.2068884192209333</v>
@@ -9906,7 +10050,7 @@
         <v>2.2300000000000004</v>
       </c>
       <c r="H12" s="0">
-        <v>1.0254364924265185</v>
+        <v>1.0254364924265176</v>
       </c>
     </row>
     <row r="13">
@@ -9929,7 +10073,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G13" s="0">
-        <v>-1.4100000000000001</v>
+        <v>-1.4099999999999966</v>
       </c>
       <c r="H13" s="0">
         <v>3.2068884192209333</v>
@@ -9955,7 +10099,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G14" s="0">
-        <v>3.1900000000000013</v>
+        <v>3.1900000000000048</v>
       </c>
       <c r="H14" s="0">
         <v>3.2068884192209333</v>
@@ -9981,7 +10125,7 @@
         <v>0.041932485418030345</v>
       </c>
       <c r="G15" s="0">
-        <v>4.0800000000000001</v>
+        <v>4.0800000000000018</v>
       </c>
       <c r="H15" s="0">
         <v>0.1677299416721216</v>
@@ -10007,7 +10151,7 @@
         <v>0.049497474683058366</v>
       </c>
       <c r="G16" s="0">
-        <v>4.3300000000000001</v>
+        <v>4.3300000000000018</v>
       </c>
       <c r="H16" s="0">
         <v>0.1979898987322341</v>
@@ -10033,7 +10177,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G17" s="0">
-        <v>0.99000000000000021</v>
+        <v>0.99000000000000199</v>
       </c>
       <c r="H17" s="0">
         <v>3.2068884192209333</v>
@@ -10085,10 +10229,10 @@
         <v>0.13435028842544403</v>
       </c>
       <c r="G19" s="0">
-        <v>0.8100000000000005</v>
+        <v>0.81000000000000227</v>
       </c>
       <c r="H19" s="0">
-        <v>0.53740115370177599</v>
+        <v>0.53740115370177477</v>
       </c>
     </row>
     <row r="20">
@@ -10111,10 +10255,10 @@
         <v>0.30405591591021547</v>
       </c>
       <c r="G20" s="0">
-        <v>-0.3100000000000005</v>
+        <v>-0.30999999999999517</v>
       </c>
       <c r="H20" s="0">
-        <v>1.2162236636408621</v>
+        <v>1.2162236636408634</v>
       </c>
     </row>
     <row r="21">
@@ -10137,7 +10281,7 @@
         <v>0.046188021535170071</v>
       </c>
       <c r="G21" s="0">
-        <v>1.5233333333333334</v>
+        <v>1.523333333333337</v>
       </c>
       <c r="H21" s="0">
         <v>0.18475208614068039</v>
@@ -10163,10 +10307,10 @@
         <v>0.09899494936611658</v>
       </c>
       <c r="G22" s="0">
-        <v>3.9499999999999975</v>
+        <v>3.9500000000000028</v>
       </c>
       <c r="H22" s="0">
-        <v>0.39597979746446571</v>
+        <v>0.39597979746446821</v>
       </c>
     </row>
     <row r="23">
@@ -10189,7 +10333,7 @@
         <v>0.3818376618407357</v>
       </c>
       <c r="G23" s="0">
-        <v>5.5499999999999989</v>
+        <v>5.5500000000000043</v>
       </c>
       <c r="H23" s="0">
         <v>1.5273506473629428</v>
@@ -10215,7 +10359,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G24" s="0">
-        <v>2.2300000000000004</v>
+        <v>2.230000000000004</v>
       </c>
       <c r="H24" s="0">
         <v>3.2068884192209333</v>
@@ -10241,10 +10385,10 @@
         <v>0.021213203435596444</v>
       </c>
       <c r="G25" s="0">
-        <v>3.7700000000000014</v>
+        <v>3.7700000000000031</v>
       </c>
       <c r="H25" s="0">
-        <v>0.08485281374238389</v>
+        <v>0.084852813742386402</v>
       </c>
     </row>
     <row r="26">
@@ -10267,7 +10411,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G26" s="0">
-        <v>6.5900000000000016</v>
+        <v>6.5900000000000034</v>
       </c>
       <c r="H26" s="0">
         <v>3.2068884192209333</v>
@@ -10293,7 +10437,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G27" s="0">
-        <v>6.4300000000000015</v>
+        <v>6.4300000000000033</v>
       </c>
       <c r="H27" s="0">
         <v>3.2068884192209333</v>
@@ -10319,10 +10463,10 @@
         <v>0.64346717087975824</v>
       </c>
       <c r="G28" s="0">
-        <v>1.5299999999999994</v>
+        <v>1.5300000000000011</v>
       </c>
       <c r="H28" s="0">
-        <v>2.5738686835190321</v>
+        <v>2.5738686835190334</v>
       </c>
     </row>
     <row r="29">
@@ -10345,7 +10489,7 @@
         <v>0.24269322199023194</v>
       </c>
       <c r="G29" s="0">
-        <v>4.2300000000000022</v>
+        <v>4.230000000000004</v>
       </c>
       <c r="H29" s="0">
         <v>0.9707728879609272</v>
@@ -10397,7 +10541,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G31" s="0">
-        <v>5.5499999999999989</v>
+        <v>5.5500000000000043</v>
       </c>
       <c r="H31" s="0">
         <v>3.2068884192209333</v>
@@ -10423,7 +10567,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G32" s="0">
-        <v>5.1100000000000012</v>
+        <v>5.110000000000003</v>
       </c>
       <c r="H32" s="0">
         <v>3.2068884192209333</v>
@@ -10449,7 +10593,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G33" s="0">
-        <v>7.6699999999999999</v>
+        <v>7.6700000000000017</v>
       </c>
       <c r="H33" s="0">
         <v>3.2068884192209333</v>
@@ -10475,10 +10619,10 @@
         <v>0.5586143571373724</v>
       </c>
       <c r="G34" s="0">
-        <v>6.0099999999999998</v>
+        <v>6.0100000000000051</v>
       </c>
       <c r="H34" s="0">
-        <v>2.2344574285494878</v>
+        <v>2.2344574285494905</v>
       </c>
     </row>
     <row r="35">
@@ -10501,7 +10645,7 @@
         <v>0.8017221048052332</v>
       </c>
       <c r="G35" s="0">
-        <v>6.6300000000000008</v>
+        <v>6.6300000000000026</v>
       </c>
       <c r="H35" s="0">
         <v>3.2068884192209333</v>
@@ -10527,7 +10671,7 @@
         <v>0.2191346617949794</v>
       </c>
       <c r="G36" s="0">
-        <v>5.4220000000000024</v>
+        <v>5.4220000000000006</v>
       </c>
       <c r="H36" s="0">
         <v>0.87653864717991792</v>

</xml_diff>